<commit_message>
exercises' excel files updated
</commit_message>
<xml_diff>
--- a/seriation-exercises/ex-2-extra_battleship-curve.xlsx
+++ b/seriation-exercises/ex-2-extra_battleship-curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0112360\Documents\____\Sagalassos\__PhD\TA\Archaeology\_class_TMP-II_2023\exercises_excel-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4B06A8-CC5B-47CC-92ED-C23608F00110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CE57D4-71B9-45D6-ABD7-D487891ED996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battleship Curve" sheetId="2" r:id="rId1"/>
@@ -65,14 +65,35 @@
     <t>end bar</t>
   </si>
   <si>
-    <t>The only cells you may modify are the ones colored in the same way as this text.</t>
+    <r>
+      <t>Modify only the cells that are highlighted in the same way as this cell. Do not cut cells, you may only copy-paste-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>values</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or type.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,8 +103,13 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="5" tint="-0.249977111117893"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,7 +117,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,18 +137,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -193,36 +224,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color theme="8" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color theme="8" tint="-0.249977111117893"/>
-      </right>
-      <top style="thick">
-        <color theme="8" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="8" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -287,46 +288,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="8" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="8" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5581,2001 +5627,2001 @@
       <c r="AG1" s="14"/>
       <c r="AH1" s="15"/>
     </row>
-    <row r="2" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
       <c r="I2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="18"/>
       <c r="P2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="18"/>
       <c r="W2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="18"/>
       <c r="AD2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AE2" s="16"/>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="16"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="18"/>
     </row>
-    <row r="3" spans="2:34" ht="58.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:34" ht="58.2" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="4" t="s">
+      <c r="K3" s="1"/>
+      <c r="L3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="4" t="s">
+      <c r="R3" s="1"/>
+      <c r="S3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="X3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="4" t="s">
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AA3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AD3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AE3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="4" t="s">
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AH3" s="5" t="s">
+      <c r="AH3" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B4" s="6">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="8">
         <v>90</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="8">
+      <c r="D4" s="1"/>
+      <c r="E4" s="3">
         <f>-ROUND(C4/2,1)</f>
         <v>-45</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="4">
         <f>ROUND(C4/2,1)</f>
         <v>45</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="8">
         <v>10</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="8">
+      <c r="K4" s="1"/>
+      <c r="L4" s="3">
         <f>-ROUND(J4/2,1)</f>
         <v>-5</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="4">
         <f>ROUND(J4/2,1)</f>
         <v>5</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="2">
         <v>1</v>
       </c>
-      <c r="Q4" s="7">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3"/>
-      <c r="S4" s="8">
+      <c r="Q4" s="8">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1"/>
+      <c r="S4" s="3">
         <f>-ROUND(Q4/2,1)</f>
         <v>0</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T4" s="4">
         <f>ROUND(Q4/2,1)</f>
         <v>0</v>
       </c>
-      <c r="W4" s="6">
+      <c r="W4" s="2">
         <v>1</v>
       </c>
-      <c r="X4" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="8">
+      <c r="X4" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="3">
         <f>-ROUND(X4/2,1)</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="9">
+      <c r="AA4" s="4">
         <f>ROUND(X4/2,1)</f>
         <v>0</v>
       </c>
-      <c r="AD4" s="6">
+      <c r="AD4" s="2">
         <v>1</v>
       </c>
-      <c r="AE4" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="8">
+      <c r="AE4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="3">
         <f>-ROUND(AE4/2,1)</f>
         <v>0</v>
       </c>
-      <c r="AH4" s="9">
+      <c r="AH4" s="4">
         <f>ROUND(AE4/2,1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
         <v>80</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="8">
+      <c r="D5" s="1"/>
+      <c r="E5" s="3">
         <f t="shared" ref="E5:E28" si="0">-ROUND(C5/2,1)</f>
         <v>-40</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="4">
         <f t="shared" ref="F5:F28" si="1">ROUND(C5/2,1)</f>
         <v>40</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="2">
         <v>2</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="8">
         <v>20</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="8">
+      <c r="K5" s="1"/>
+      <c r="L5" s="3">
         <f t="shared" ref="L5:L22" si="2">-J5/2</f>
         <v>-10</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="4">
         <f t="shared" ref="M5:M22" si="3">J5/2</f>
         <v>10</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="2">
         <v>2</v>
       </c>
-      <c r="Q5" s="7">
-        <v>0</v>
-      </c>
-      <c r="R5" s="3"/>
-      <c r="S5" s="8">
+      <c r="Q5" s="8">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="3">
         <f t="shared" ref="S5:S28" si="4">-ROUND(Q5/2,1)</f>
         <v>0</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="4">
         <f t="shared" ref="T5:T28" si="5">ROUND(Q5/2,1)</f>
         <v>0</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W5" s="2">
         <v>2</v>
       </c>
-      <c r="X5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="8">
+      <c r="X5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="3">
         <f t="shared" ref="Z5:Z28" si="6">-ROUND(X5/2,1)</f>
         <v>0</v>
       </c>
-      <c r="AA5" s="9">
+      <c r="AA5" s="4">
         <f t="shared" ref="AA5:AA28" si="7">ROUND(X5/2,1)</f>
         <v>0</v>
       </c>
-      <c r="AD5" s="6">
+      <c r="AD5" s="2">
         <v>2</v>
       </c>
-      <c r="AE5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="8">
+      <c r="AE5" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="3">
         <f t="shared" ref="AG5:AG27" si="8">-ROUND(AE5/2,1)</f>
         <v>0</v>
       </c>
-      <c r="AH5" s="9">
+      <c r="AH5" s="4">
         <f t="shared" ref="AH5:AH27" si="9">ROUND(AE5/2,1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B6" s="6">
+      <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="8">
         <v>70</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="8">
+      <c r="D6" s="1"/>
+      <c r="E6" s="3">
         <f t="shared" si="0"/>
         <v>-35</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="4">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="2">
         <v>3</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="8">
         <v>30</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="8">
+      <c r="K6" s="1"/>
+      <c r="L6" s="3">
         <f t="shared" si="2"/>
         <v>-15</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="4">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="2">
         <v>3</v>
       </c>
-      <c r="Q6" s="7">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3"/>
-      <c r="S6" s="8">
+      <c r="Q6" s="8">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1"/>
+      <c r="S6" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W6" s="6">
+      <c r="W6" s="2">
         <v>3</v>
       </c>
-      <c r="X6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="8">
+      <c r="X6" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="9">
+      <c r="AA6" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="6">
+      <c r="AD6" s="2">
         <v>3</v>
       </c>
-      <c r="AE6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="8">
+      <c r="AE6" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH6" s="9">
+      <c r="AH6" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>4</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="8">
         <v>65</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="8">
+      <c r="D7" s="1"/>
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>-32.5</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="4">
         <f t="shared" si="1"/>
         <v>32.5</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="2">
         <v>4</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="8">
         <v>30</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="8">
+      <c r="K7" s="1"/>
+      <c r="L7" s="3">
         <f t="shared" si="2"/>
         <v>-15</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="4">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="2">
         <v>4</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="8">
         <v>5</v>
       </c>
-      <c r="R7" s="3"/>
-      <c r="S7" s="8">
+      <c r="R7" s="1"/>
+      <c r="S7" s="3">
         <f t="shared" si="4"/>
         <v>-2.5</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="4">
         <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
-      <c r="W7" s="6">
+      <c r="W7" s="2">
         <v>4</v>
       </c>
-      <c r="X7" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="8">
+      <c r="X7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA7" s="9">
+      <c r="AA7" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="6">
+      <c r="AD7" s="2">
         <v>4</v>
       </c>
-      <c r="AE7" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="8">
+      <c r="AE7" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH7" s="9">
+      <c r="AH7" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B8" s="6">
+      <c r="B8" s="2">
         <v>5</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="8">
         <v>50</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="8">
+      <c r="D8" s="1"/>
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>-25</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="4">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="2">
         <v>5</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="8">
         <v>40</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="8">
+      <c r="K8" s="1"/>
+      <c r="L8" s="3">
         <f t="shared" si="2"/>
         <v>-20</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="4">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="2">
         <v>5</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="8">
         <v>10</v>
       </c>
-      <c r="R8" s="3"/>
-      <c r="S8" s="8">
+      <c r="R8" s="1"/>
+      <c r="S8" s="3">
         <f t="shared" si="4"/>
         <v>-5</v>
       </c>
-      <c r="T8" s="9">
+      <c r="T8" s="4">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="W8" s="6">
+      <c r="W8" s="2">
         <v>5</v>
       </c>
-      <c r="X8" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="8">
+      <c r="X8" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA8" s="9">
+      <c r="AA8" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD8" s="6">
+      <c r="AD8" s="2">
         <v>5</v>
       </c>
-      <c r="AE8" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="8">
+      <c r="AE8" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH8" s="9">
+      <c r="AH8" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <v>30</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="8">
+      <c r="D9" s="1"/>
+      <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>-15</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="4">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="2">
         <v>6</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="8">
         <v>50</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="8">
+      <c r="K9" s="1"/>
+      <c r="L9" s="3">
         <f t="shared" si="2"/>
         <v>-25</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="4">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="2">
         <v>6</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="8">
         <v>20</v>
       </c>
-      <c r="R9" s="3"/>
-      <c r="S9" s="8">
+      <c r="R9" s="1"/>
+      <c r="S9" s="3">
         <f t="shared" si="4"/>
         <v>-10</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="4">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="W9" s="6">
+      <c r="W9" s="2">
         <v>6</v>
       </c>
-      <c r="X9" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="8">
+      <c r="X9" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA9" s="9">
+      <c r="AA9" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD9" s="6">
+      <c r="AD9" s="2">
         <v>6</v>
       </c>
-      <c r="AE9" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="8">
+      <c r="AE9" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH9" s="9">
+      <c r="AH9" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B10" s="6">
+      <c r="B10" s="2">
         <v>7</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <v>10</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="8">
+      <c r="D10" s="1"/>
+      <c r="E10" s="3">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="2">
         <v>7</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="8">
         <v>60</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="8">
+      <c r="K10" s="1"/>
+      <c r="L10" s="3">
         <f t="shared" si="2"/>
         <v>-30</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="4">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="2">
         <v>7</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="8">
         <v>30</v>
       </c>
-      <c r="R10" s="3"/>
-      <c r="S10" s="8">
+      <c r="R10" s="1"/>
+      <c r="S10" s="3">
         <f t="shared" si="4"/>
         <v>-15</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="4">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="W10" s="6">
+      <c r="W10" s="2">
         <v>7</v>
       </c>
-      <c r="X10" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="8">
+      <c r="X10" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA10" s="9">
+      <c r="AA10" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD10" s="6">
+      <c r="AD10" s="2">
         <v>7</v>
       </c>
-      <c r="AE10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="8">
+      <c r="AE10" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH10" s="9">
+      <c r="AH10" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B11" s="6">
+      <c r="B11" s="2">
         <v>8</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="8">
         <v>10</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="8">
+      <c r="D11" s="1"/>
+      <c r="E11" s="3">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="2">
         <v>8</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="8">
         <v>60</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="8">
+      <c r="K11" s="1"/>
+      <c r="L11" s="3">
         <f t="shared" si="2"/>
         <v>-30</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="4">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="P11" s="6">
+      <c r="P11" s="2">
         <v>8</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q11" s="8">
         <v>30</v>
       </c>
-      <c r="R11" s="3"/>
-      <c r="S11" s="8">
+      <c r="R11" s="1"/>
+      <c r="S11" s="3">
         <f t="shared" si="4"/>
         <v>-15</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="4">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="W11" s="6">
+      <c r="W11" s="2">
         <v>8</v>
       </c>
-      <c r="X11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="8">
+      <c r="X11" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA11" s="9">
+      <c r="AA11" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD11" s="6">
+      <c r="AD11" s="2">
         <v>8</v>
       </c>
-      <c r="AE11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="8">
+      <c r="AE11" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH11" s="9">
+      <c r="AH11" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B12" s="6">
+      <c r="B12" s="2">
         <v>9</v>
       </c>
-      <c r="C12" s="7">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="8">
+      <c r="C12" s="8">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="2">
         <v>9</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="8">
         <v>75</v>
       </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="8">
+      <c r="K12" s="1"/>
+      <c r="L12" s="3">
         <f t="shared" si="2"/>
         <v>-37.5</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="4">
         <f t="shared" si="3"/>
         <v>37.5</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="2">
         <v>9</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="8">
         <v>25</v>
       </c>
-      <c r="R12" s="3"/>
-      <c r="S12" s="8">
+      <c r="R12" s="1"/>
+      <c r="S12" s="3">
         <f t="shared" si="4"/>
         <v>-12.5</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="4">
         <f t="shared" si="5"/>
         <v>12.5</v>
       </c>
-      <c r="W12" s="6">
+      <c r="W12" s="2">
         <v>9</v>
       </c>
-      <c r="X12" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="8">
+      <c r="X12" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA12" s="9">
+      <c r="AA12" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD12" s="6">
+      <c r="AD12" s="2">
         <v>9</v>
       </c>
-      <c r="AE12" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="3"/>
-      <c r="AG12" s="8">
+      <c r="AE12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH12" s="9">
+      <c r="AH12" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B13" s="6">
+      <c r="B13" s="2">
         <v>10</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="8">
         <v>10</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="8">
+      <c r="D13" s="1"/>
+      <c r="E13" s="3">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="2">
         <v>10</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="8">
         <v>80</v>
       </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="8">
+      <c r="K13" s="1"/>
+      <c r="L13" s="3">
         <f t="shared" si="2"/>
         <v>-40</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="4">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="2">
         <v>10</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q13" s="8">
         <v>5</v>
       </c>
-      <c r="R13" s="3"/>
-      <c r="S13" s="8">
+      <c r="R13" s="1"/>
+      <c r="S13" s="3">
         <f t="shared" si="4"/>
         <v>-2.5</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="4">
         <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
-      <c r="W13" s="6">
+      <c r="W13" s="2">
         <v>10</v>
       </c>
-      <c r="X13" s="7">
+      <c r="X13" s="8">
         <v>5</v>
       </c>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="8">
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="3">
         <f t="shared" si="6"/>
         <v>-2.5</v>
       </c>
-      <c r="AA13" s="9">
+      <c r="AA13" s="4">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
-      <c r="AD13" s="6">
+      <c r="AD13" s="2">
         <v>10</v>
       </c>
-      <c r="AE13" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="3"/>
-      <c r="AG13" s="8">
+      <c r="AE13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH13" s="9">
+      <c r="AH13" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B14" s="6">
+      <c r="B14" s="2">
         <v>11</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="8">
         <v>10</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="8">
+      <c r="D14" s="1"/>
+      <c r="E14" s="3">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="2">
         <v>11</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="8">
         <v>90</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="8">
+      <c r="K14" s="1"/>
+      <c r="L14" s="3">
         <f t="shared" si="2"/>
         <v>-45</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="4">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P14" s="2">
         <v>11</v>
       </c>
-      <c r="Q14" s="7">
-        <v>0</v>
-      </c>
-      <c r="R14" s="3"/>
-      <c r="S14" s="8">
+      <c r="Q14" s="8">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1"/>
+      <c r="S14" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T14" s="9">
+      <c r="T14" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W14" s="6">
+      <c r="W14" s="2">
         <v>11</v>
       </c>
-      <c r="X14" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="8">
+      <c r="X14" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA14" s="9">
+      <c r="AA14" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD14" s="6">
+      <c r="AD14" s="2">
         <v>11</v>
       </c>
-      <c r="AE14" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="3"/>
-      <c r="AG14" s="8">
+      <c r="AE14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH14" s="9">
+      <c r="AH14" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B15" s="6">
+      <c r="B15" s="2">
         <v>12</v>
       </c>
-      <c r="C15" s="7">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="8">
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="2">
         <v>12</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="8">
         <v>90</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="8">
+      <c r="K15" s="1"/>
+      <c r="L15" s="3">
         <f t="shared" si="2"/>
         <v>-45</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="4">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="P15" s="6">
+      <c r="P15" s="2">
         <v>12</v>
       </c>
-      <c r="Q15" s="7">
-        <v>0</v>
-      </c>
-      <c r="R15" s="3"/>
-      <c r="S15" s="8">
+      <c r="Q15" s="8">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1"/>
+      <c r="S15" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W15" s="6">
+      <c r="W15" s="2">
         <v>12</v>
       </c>
-      <c r="X15" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="8">
+      <c r="X15" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA15" s="9">
+      <c r="AA15" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD15" s="6">
+      <c r="AD15" s="2">
         <v>12</v>
       </c>
-      <c r="AE15" s="7">
+      <c r="AE15" s="8">
         <v>10</v>
       </c>
-      <c r="AF15" s="3"/>
-      <c r="AG15" s="8">
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="3">
         <f t="shared" si="8"/>
         <v>-5</v>
       </c>
-      <c r="AH15" s="9">
+      <c r="AH15" s="4">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B16" s="6">
+      <c r="B16" s="2">
         <v>13</v>
       </c>
-      <c r="C16" s="7">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="8">
+      <c r="C16" s="8">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="2">
         <v>13</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="8">
         <v>80</v>
       </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="8">
+      <c r="K16" s="1"/>
+      <c r="L16" s="3">
         <f t="shared" si="2"/>
         <v>-40</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="4">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="P16" s="6">
+      <c r="P16" s="2">
         <v>13</v>
       </c>
-      <c r="Q16" s="7">
-        <v>0</v>
-      </c>
-      <c r="R16" s="3"/>
-      <c r="S16" s="8">
+      <c r="Q16" s="8">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1"/>
+      <c r="S16" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T16" s="9">
+      <c r="T16" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W16" s="6">
+      <c r="W16" s="2">
         <v>13</v>
       </c>
-      <c r="X16" s="7">
+      <c r="X16" s="8">
         <v>5</v>
       </c>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="8">
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="3">
         <f t="shared" si="6"/>
         <v>-2.5</v>
       </c>
-      <c r="AA16" s="9">
+      <c r="AA16" s="4">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
-      <c r="AD16" s="6">
+      <c r="AD16" s="2">
         <v>13</v>
       </c>
-      <c r="AE16" s="7">
+      <c r="AE16" s="8">
         <v>15</v>
       </c>
-      <c r="AF16" s="3"/>
-      <c r="AG16" s="8">
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="3">
         <f t="shared" si="8"/>
         <v>-7.5</v>
       </c>
-      <c r="AH16" s="9">
+      <c r="AH16" s="4">
         <f t="shared" si="9"/>
         <v>7.5</v>
       </c>
     </row>
     <row r="17" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B17" s="6">
+      <c r="B17" s="2">
         <v>14</v>
       </c>
-      <c r="C17" s="7">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="8">
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="2">
         <v>14</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="8">
         <v>70</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="8">
+      <c r="K17" s="1"/>
+      <c r="L17" s="3">
         <f t="shared" si="2"/>
         <v>-35</v>
       </c>
-      <c r="M17" s="9">
+      <c r="M17" s="4">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="P17" s="6">
+      <c r="P17" s="2">
         <v>14</v>
       </c>
-      <c r="Q17" s="7">
-        <v>0</v>
-      </c>
-      <c r="R17" s="3"/>
-      <c r="S17" s="8">
+      <c r="Q17" s="8">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1"/>
+      <c r="S17" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T17" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W17" s="6">
+      <c r="W17" s="2">
         <v>14</v>
       </c>
-      <c r="X17" s="7">
+      <c r="X17" s="8">
         <v>10</v>
       </c>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="8">
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="3">
         <f t="shared" si="6"/>
         <v>-5</v>
       </c>
-      <c r="AA17" s="9">
+      <c r="AA17" s="4">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="AD17" s="6">
+      <c r="AD17" s="2">
         <v>14</v>
       </c>
-      <c r="AE17" s="7">
+      <c r="AE17" s="8">
         <v>20</v>
       </c>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="8">
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="3">
         <f t="shared" si="8"/>
         <v>-10</v>
       </c>
-      <c r="AH17" s="9">
+      <c r="AH17" s="4">
         <f t="shared" si="9"/>
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B18" s="6">
+      <c r="B18" s="2">
         <v>15</v>
       </c>
-      <c r="C18" s="7">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="8">
+      <c r="C18" s="8">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="2">
         <v>15</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="8">
         <v>50</v>
       </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="8">
+      <c r="K18" s="1"/>
+      <c r="L18" s="3">
         <f t="shared" si="2"/>
         <v>-25</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="4">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="P18" s="6">
+      <c r="P18" s="2">
         <v>15</v>
       </c>
-      <c r="Q18" s="7">
-        <v>0</v>
-      </c>
-      <c r="R18" s="3"/>
-      <c r="S18" s="8">
+      <c r="Q18" s="8">
+        <v>0</v>
+      </c>
+      <c r="R18" s="1"/>
+      <c r="S18" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T18" s="9">
+      <c r="T18" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W18" s="6">
+      <c r="W18" s="2">
         <v>15</v>
       </c>
-      <c r="X18" s="7">
+      <c r="X18" s="8">
         <v>25</v>
       </c>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="8">
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="3">
         <f t="shared" si="6"/>
         <v>-12.5</v>
       </c>
-      <c r="AA18" s="9">
+      <c r="AA18" s="4">
         <f t="shared" si="7"/>
         <v>12.5</v>
       </c>
-      <c r="AD18" s="6">
+      <c r="AD18" s="2">
         <v>15</v>
       </c>
-      <c r="AE18" s="7">
+      <c r="AE18" s="8">
         <v>25</v>
       </c>
-      <c r="AF18" s="3"/>
-      <c r="AG18" s="8">
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="3">
         <f t="shared" si="8"/>
         <v>-12.5</v>
       </c>
-      <c r="AH18" s="9">
+      <c r="AH18" s="4">
         <f t="shared" si="9"/>
         <v>12.5</v>
       </c>
     </row>
     <row r="19" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B19" s="6">
+      <c r="B19" s="2">
         <v>16</v>
       </c>
-      <c r="C19" s="7">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="8">
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="2">
         <v>16</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="8">
         <v>40</v>
       </c>
-      <c r="K19" s="3"/>
-      <c r="L19" s="8">
+      <c r="K19" s="1"/>
+      <c r="L19" s="3">
         <f t="shared" si="2"/>
         <v>-20</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="4">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="P19" s="6">
+      <c r="P19" s="2">
         <v>16</v>
       </c>
-      <c r="Q19" s="7">
-        <v>0</v>
-      </c>
-      <c r="R19" s="3"/>
-      <c r="S19" s="8">
+      <c r="Q19" s="8">
+        <v>0</v>
+      </c>
+      <c r="R19" s="1"/>
+      <c r="S19" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T19" s="9">
+      <c r="T19" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W19" s="6">
+      <c r="W19" s="2">
         <v>16</v>
       </c>
-      <c r="X19" s="7">
+      <c r="X19" s="8">
         <v>20</v>
       </c>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="8">
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="3">
         <f t="shared" si="6"/>
         <v>-10</v>
       </c>
-      <c r="AA19" s="9">
+      <c r="AA19" s="4">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="AD19" s="6">
+      <c r="AD19" s="2">
         <v>16</v>
       </c>
-      <c r="AE19" s="7">
+      <c r="AE19" s="8">
         <v>40</v>
       </c>
-      <c r="AF19" s="3"/>
-      <c r="AG19" s="8">
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="3">
         <f t="shared" si="8"/>
         <v>-20</v>
       </c>
-      <c r="AH19" s="9">
+      <c r="AH19" s="4">
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B20" s="6">
+      <c r="B20" s="2">
         <v>17</v>
       </c>
-      <c r="C20" s="7">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="8">
+      <c r="C20" s="8">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="2">
         <v>17</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="8">
         <v>30</v>
       </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="8">
+      <c r="K20" s="1"/>
+      <c r="L20" s="3">
         <f t="shared" si="2"/>
         <v>-15</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="4">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="P20" s="6">
+      <c r="P20" s="2">
         <v>17</v>
       </c>
-      <c r="Q20" s="7">
-        <v>0</v>
-      </c>
-      <c r="R20" s="3"/>
-      <c r="S20" s="8">
+      <c r="Q20" s="8">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1"/>
+      <c r="S20" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T20" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W20" s="6">
+      <c r="W20" s="2">
         <v>17</v>
       </c>
-      <c r="X20" s="7">
+      <c r="X20" s="8">
         <v>20</v>
       </c>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="8">
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="3">
         <f t="shared" si="6"/>
         <v>-10</v>
       </c>
-      <c r="AA20" s="9">
+      <c r="AA20" s="4">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="AD20" s="6">
+      <c r="AD20" s="2">
         <v>17</v>
       </c>
-      <c r="AE20" s="7">
+      <c r="AE20" s="8">
         <v>50</v>
       </c>
-      <c r="AF20" s="3"/>
-      <c r="AG20" s="8">
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="3">
         <f t="shared" si="8"/>
         <v>-25</v>
       </c>
-      <c r="AH20" s="9">
+      <c r="AH20" s="4">
         <f t="shared" si="9"/>
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B21" s="6">
+      <c r="B21" s="2">
         <v>18</v>
       </c>
-      <c r="C21" s="7">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="8">
+      <c r="C21" s="8">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="2">
         <v>18</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="8">
         <v>10</v>
       </c>
-      <c r="K21" s="3"/>
-      <c r="L21" s="8">
+      <c r="K21" s="1"/>
+      <c r="L21" s="3">
         <f t="shared" si="2"/>
         <v>-5</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M21" s="4">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="P21" s="6">
+      <c r="P21" s="2">
         <v>18</v>
       </c>
-      <c r="Q21" s="7">
-        <v>0</v>
-      </c>
-      <c r="R21" s="3"/>
-      <c r="S21" s="8">
+      <c r="Q21" s="8">
+        <v>0</v>
+      </c>
+      <c r="R21" s="1"/>
+      <c r="S21" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T21" s="9">
+      <c r="T21" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W21" s="6">
+      <c r="W21" s="2">
         <v>18</v>
       </c>
-      <c r="X21" s="7">
+      <c r="X21" s="8">
         <v>30</v>
       </c>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="8">
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="3">
         <f t="shared" si="6"/>
         <v>-15</v>
       </c>
-      <c r="AA21" s="9">
+      <c r="AA21" s="4">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
-      <c r="AD21" s="6">
+      <c r="AD21" s="2">
         <v>18</v>
       </c>
-      <c r="AE21" s="7">
+      <c r="AE21" s="8">
         <v>60</v>
       </c>
-      <c r="AF21" s="3"/>
-      <c r="AG21" s="8">
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="3">
         <f t="shared" si="8"/>
         <v>-30</v>
       </c>
-      <c r="AH21" s="9">
+      <c r="AH21" s="4">
         <f t="shared" si="9"/>
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B22" s="6">
+      <c r="B22" s="2">
         <v>19</v>
       </c>
-      <c r="C22" s="7">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="8">
+      <c r="C22" s="8">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="2">
         <v>19</v>
       </c>
-      <c r="J22" s="7">
-        <v>0</v>
-      </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="8">
+      <c r="J22" s="8">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M22" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P22" s="6">
+      <c r="P22" s="2">
         <v>19</v>
       </c>
-      <c r="Q22" s="7">
-        <v>0</v>
-      </c>
-      <c r="R22" s="3"/>
-      <c r="S22" s="8">
+      <c r="Q22" s="8">
+        <v>0</v>
+      </c>
+      <c r="R22" s="1"/>
+      <c r="S22" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T22" s="9">
+      <c r="T22" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W22" s="6">
+      <c r="W22" s="2">
         <v>19</v>
       </c>
-      <c r="X22" s="7">
+      <c r="X22" s="8">
         <v>20</v>
       </c>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="8">
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="3">
         <f t="shared" si="6"/>
         <v>-10</v>
       </c>
-      <c r="AA22" s="9">
+      <c r="AA22" s="4">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="AD22" s="6">
+      <c r="AD22" s="2">
         <v>19</v>
       </c>
-      <c r="AE22" s="7">
+      <c r="AE22" s="8">
         <v>80</v>
       </c>
-      <c r="AF22" s="3"/>
-      <c r="AG22" s="8">
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="3">
         <f t="shared" si="8"/>
         <v>-40</v>
       </c>
-      <c r="AH22" s="9">
+      <c r="AH22" s="4">
         <f t="shared" si="9"/>
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B23" s="6">
+      <c r="B23" s="2">
         <v>20</v>
       </c>
-      <c r="C23" s="7">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="8">
+      <c r="C23" s="8">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="3">
         <f t="shared" ref="E23:E27" si="10">-ROUND(C23/2,1)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="4">
         <f t="shared" ref="F23:F27" si="11">ROUND(C23/2,1)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="2">
         <v>20</v>
       </c>
-      <c r="J23" s="7">
-        <v>0</v>
-      </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="8">
+      <c r="J23" s="8">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="L23" s="3">
         <f t="shared" ref="L23:L27" si="12">-ROUND(J23/2,1)</f>
         <v>0</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M23" s="4">
         <f t="shared" ref="M23:M27" si="13">ROUND(J23/2,1)</f>
         <v>0</v>
       </c>
-      <c r="P23" s="6">
+      <c r="P23" s="2">
         <v>20</v>
       </c>
-      <c r="Q23" s="7">
-        <v>0</v>
-      </c>
-      <c r="R23" s="3"/>
-      <c r="S23" s="8">
+      <c r="Q23" s="8">
+        <v>0</v>
+      </c>
+      <c r="R23" s="1"/>
+      <c r="S23" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T23" s="9">
+      <c r="T23" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W23" s="6">
+      <c r="W23" s="2">
         <v>20</v>
       </c>
-      <c r="X23" s="7">
+      <c r="X23" s="8">
         <v>15</v>
       </c>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="8">
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="3">
         <f t="shared" si="6"/>
         <v>-7.5</v>
       </c>
-      <c r="AA23" s="9">
+      <c r="AA23" s="4">
         <f t="shared" si="7"/>
         <v>7.5</v>
       </c>
-      <c r="AD23" s="6">
+      <c r="AD23" s="2">
         <v>20</v>
       </c>
-      <c r="AE23" s="7">
+      <c r="AE23" s="8">
         <v>85</v>
       </c>
-      <c r="AF23" s="3"/>
-      <c r="AG23" s="8">
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="3">
         <f t="shared" si="8"/>
         <v>-42.5</v>
       </c>
-      <c r="AH23" s="9">
+      <c r="AH23" s="4">
         <f t="shared" si="9"/>
         <v>42.5</v>
       </c>
     </row>
     <row r="24" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B24" s="6">
+      <c r="B24" s="2">
         <v>21</v>
       </c>
-      <c r="C24" s="7">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="8">
+      <c r="C24" s="8">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="2">
         <v>21</v>
       </c>
-      <c r="J24" s="7">
-        <v>0</v>
-      </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="8">
+      <c r="J24" s="8">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="M24" s="9">
+      <c r="M24" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="P24" s="6">
+      <c r="P24" s="2">
         <v>21</v>
       </c>
-      <c r="Q24" s="7">
-        <v>0</v>
-      </c>
-      <c r="R24" s="3"/>
-      <c r="S24" s="8">
+      <c r="Q24" s="8">
+        <v>0</v>
+      </c>
+      <c r="R24" s="1"/>
+      <c r="S24" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T24" s="9">
+      <c r="T24" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W24" s="6">
+      <c r="W24" s="2">
         <v>21</v>
       </c>
-      <c r="X24" s="7">
+      <c r="X24" s="8">
         <v>10</v>
       </c>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="8">
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="3">
         <f t="shared" si="6"/>
         <v>-5</v>
       </c>
-      <c r="AA24" s="9">
+      <c r="AA24" s="4">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="AD24" s="6">
+      <c r="AD24" s="2">
         <v>21</v>
       </c>
-      <c r="AE24" s="7">
+      <c r="AE24" s="8">
         <v>90</v>
       </c>
-      <c r="AF24" s="3"/>
-      <c r="AG24" s="8">
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="3">
         <f t="shared" si="8"/>
         <v>-45</v>
       </c>
-      <c r="AH24" s="9">
+      <c r="AH24" s="4">
         <f t="shared" si="9"/>
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B25" s="6">
+      <c r="B25" s="2">
         <v>22</v>
       </c>
-      <c r="C25" s="7">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="8">
+      <c r="C25" s="8">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="2">
         <v>22</v>
       </c>
-      <c r="J25" s="7">
-        <v>0</v>
-      </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="8">
+      <c r="J25" s="8">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="M25" s="9">
+      <c r="M25" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="P25" s="6">
+      <c r="P25" s="2">
         <v>22</v>
       </c>
-      <c r="Q25" s="7">
-        <v>0</v>
-      </c>
-      <c r="R25" s="3"/>
-      <c r="S25" s="8">
+      <c r="Q25" s="8">
+        <v>0</v>
+      </c>
+      <c r="R25" s="1"/>
+      <c r="S25" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T25" s="9">
+      <c r="T25" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W25" s="6">
+      <c r="W25" s="2">
         <v>22</v>
       </c>
-      <c r="X25" s="7">
+      <c r="X25" s="8">
         <v>5</v>
       </c>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="8">
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="3">
         <f t="shared" si="6"/>
         <v>-2.5</v>
       </c>
-      <c r="AA25" s="9">
+      <c r="AA25" s="4">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
-      <c r="AD25" s="6">
+      <c r="AD25" s="2">
         <v>22</v>
       </c>
-      <c r="AE25" s="7">
+      <c r="AE25" s="8">
         <v>95</v>
       </c>
-      <c r="AF25" s="3"/>
-      <c r="AG25" s="8">
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="3">
         <f t="shared" si="8"/>
         <v>-47.5</v>
       </c>
-      <c r="AH25" s="9">
+      <c r="AH25" s="4">
         <f t="shared" si="9"/>
         <v>47.5</v>
       </c>
     </row>
     <row r="26" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B26" s="6">
+      <c r="B26" s="2">
         <v>23</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="8">
+      <c r="C26" s="8"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="2">
         <v>23</v>
       </c>
-      <c r="J26" s="7"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="8">
+      <c r="J26" s="8"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="M26" s="9">
+      <c r="M26" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="P26" s="6">
+      <c r="P26" s="2">
         <v>23</v>
       </c>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="8">
+      <c r="Q26" s="8"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T26" s="9">
+      <c r="T26" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W26" s="6">
+      <c r="W26" s="2">
         <v>23</v>
       </c>
-      <c r="X26" s="7"/>
-      <c r="Y26" s="3"/>
-      <c r="Z26" s="8">
+      <c r="X26" s="8"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA26" s="9">
+      <c r="AA26" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD26" s="6">
+      <c r="AD26" s="2">
         <v>23</v>
       </c>
-      <c r="AE26" s="7"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="8">
+      <c r="AE26" s="8"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH26" s="9">
+      <c r="AH26" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B27" s="6">
+      <c r="B27" s="2">
         <v>24</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="8">
+      <c r="C27" s="8"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="2">
         <v>24</v>
       </c>
-      <c r="J27" s="7"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="8">
+      <c r="J27" s="8"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="3">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="M27" s="9">
+      <c r="M27" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="P27" s="6">
+      <c r="P27" s="2">
         <v>24</v>
       </c>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="8">
+      <c r="Q27" s="8"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T27" s="9">
+      <c r="T27" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W27" s="6">
+      <c r="W27" s="2">
         <v>24</v>
       </c>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="3"/>
-      <c r="Z27" s="8">
+      <c r="X27" s="8"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA27" s="9">
+      <c r="AA27" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD27" s="6">
+      <c r="AD27" s="2">
         <v>24</v>
       </c>
-      <c r="AE27" s="7"/>
-      <c r="AF27" s="3"/>
-      <c r="AG27" s="8">
+      <c r="AE27" s="8"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="3">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH27" s="9">
+      <c r="AH27" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="6">
+      <c r="B28" s="2">
         <v>25</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11">
+      <c r="C28" s="8"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="2">
         <v>25</v>
       </c>
-      <c r="J28" s="7"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="11">
+      <c r="J28" s="8"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="6">
         <f t="shared" ref="L28" si="14">-ROUND(J28/2,1)</f>
         <v>0</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="7">
         <f t="shared" ref="M28" si="15">ROUND(J28/2,1)</f>
         <v>0</v>
       </c>
-      <c r="P28" s="6">
+      <c r="P28" s="2">
         <v>25</v>
       </c>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="11">
+      <c r="Q28" s="8"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T28" s="12">
+      <c r="T28" s="7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W28" s="6">
+      <c r="W28" s="2">
         <v>25</v>
       </c>
-      <c r="X28" s="7"/>
-      <c r="Y28" s="10"/>
-      <c r="Z28" s="11">
+      <c r="X28" s="8"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA28" s="12">
+      <c r="AA28" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD28" s="6">
+      <c r="AD28" s="2">
         <v>25</v>
       </c>
-      <c r="AE28" s="7"/>
-      <c r="AF28" s="10"/>
-      <c r="AG28" s="11">
+      <c r="AE28" s="8"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="6">
         <f t="shared" ref="AG28" si="16">-ROUND(AE28/2,1)</f>
         <v>0</v>
       </c>
-      <c r="AH28" s="12">
+      <c r="AH28" s="7">
         <f t="shared" ref="AH28" si="17">ROUND(AE28/2,1)</f>
         <v>0</v>
       </c>

</xml_diff>